<commit_message>
Some transcription errors were corrected
</commit_message>
<xml_diff>
--- a/res/rasgos.xlsx
+++ b/res/rasgos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vocales" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,14 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="66">
   <si>
     <t xml:space="preserve">i</t>
   </si>
   <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
     <t xml:space="preserve">u</t>
   </si>
   <si>
@@ -92,7 +89,7 @@
     <t xml:space="preserve">?</t>
   </si>
   <si>
-    <t xml:space="preserve">p\</t>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
@@ -122,13 +119,13 @@
     <t xml:space="preserve">h</t>
   </si>
   <si>
-    <t xml:space="preserve">ts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dZ</t>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
@@ -137,7 +134,7 @@
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve">J</t>
+    <t xml:space="preserve">ñ</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -146,15 +143,15 @@
     <t xml:space="preserve">r</t>
   </si>
   <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
     <t xml:space="preserve">l</t>
   </si>
   <si>
     <t xml:space="preserve">L</t>
   </si>
   <si>
-    <t xml:space="preserve">ɺ</t>
-  </si>
-  <si>
     <t xml:space="preserve">SONORANT</t>
   </si>
   <si>
@@ -180,6 +177,48 @@
   </si>
   <si>
     <t xml:space="preserve">DORSAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʔ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ɸ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">β</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ɬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ʒ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ɣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t͡s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t͡ʃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d͡ʒ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ɲ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ɾ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ɽ</t>
   </si>
 </sst>
 </file>
@@ -289,241 +328,224 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="5.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H1" s="1" t="n">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -542,93 +564,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="2" style="1" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="2" style="1" width="4.97"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>4</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>40</v>
@@ -639,836 +661,894 @@
       <c r="AC1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="AD5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="AD7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD10" s="1" t="s">
-        <v>11</v>
+      <c r="I13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Chibchan Tree finished, at last
</commit_message>
<xml_diff>
--- a/res/rasgos.xlsx
+++ b/res/rasgos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vocales" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="52">
   <si>
     <t xml:space="preserve">i</t>
   </si>
@@ -177,48 +177,6 @@
   </si>
   <si>
     <t xml:space="preserve">DORSAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ʔ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ɸ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">β</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ɬ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ʃ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ʒ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ɣ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t͡s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t͡ʃ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d͡ʒ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ɲ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ŋ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ɾ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ɽ</t>
   </si>
 </sst>
 </file>
@@ -330,8 +288,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -566,8 +524,8 @@
   </sheetPr>
   <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="AD1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1465,92 +1423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>